<commit_message>
Add Specification for GenericRepository and images
</commit_message>
<xml_diff>
--- a/Infrastructure/Data/SeedingData/ProductECommerce.xlsx
+++ b/Infrastructure/Data/SeedingData/ProductECommerce.xlsx
@@ -545,304 +545,304 @@
     <t>pictureUrl</t>
   </si>
   <si>
-    <t>Images/Product/product 1</t>
-  </si>
-  <si>
-    <t>Images/Product/product 2</t>
-  </si>
-  <si>
-    <t>Images/Product/product 3</t>
-  </si>
-  <si>
-    <t>Images/Product/product 4</t>
-  </si>
-  <si>
-    <t>Images/Product/product 5</t>
-  </si>
-  <si>
-    <t>Images/Product/product 6</t>
-  </si>
-  <si>
-    <t>Images/Product/product 7</t>
-  </si>
-  <si>
-    <t>Images/Product/product 8</t>
-  </si>
-  <si>
-    <t>Images/Product/product 9</t>
-  </si>
-  <si>
-    <t>Images/Product/product 10</t>
-  </si>
-  <si>
-    <t>Images/Product/product 11</t>
-  </si>
-  <si>
-    <t>Images/Product/product 12</t>
-  </si>
-  <si>
-    <t>Images/Product/product 13</t>
-  </si>
-  <si>
-    <t>Images/Product/product 14</t>
-  </si>
-  <si>
-    <t>Images/Product/product 15</t>
-  </si>
-  <si>
-    <t>Images/Product/product 16</t>
-  </si>
-  <si>
-    <t>Images/Product/product 17</t>
-  </si>
-  <si>
-    <t>Images/Product/product 18</t>
-  </si>
-  <si>
-    <t>Images/Product/product 19</t>
-  </si>
-  <si>
-    <t>Images/Product/product 20</t>
-  </si>
-  <si>
-    <t>Images/Product/product 21</t>
-  </si>
-  <si>
-    <t>Images/Product/product 22</t>
-  </si>
-  <si>
-    <t>Images/Product/product 23</t>
-  </si>
-  <si>
-    <t>Images/Product/product 24</t>
-  </si>
-  <si>
-    <t>Images/Product/product 25</t>
-  </si>
-  <si>
-    <t>Images/Product/product 26</t>
-  </si>
-  <si>
-    <t>Images/Product/product 27</t>
-  </si>
-  <si>
-    <t>Images/Product/product 28</t>
-  </si>
-  <si>
-    <t>Images/Product/product 29</t>
-  </si>
-  <si>
-    <t>Images/Product/product 30</t>
-  </si>
-  <si>
-    <t>Images/Product/product 31</t>
-  </si>
-  <si>
-    <t>Images/Product/product 32</t>
-  </si>
-  <si>
-    <t>Images/Product/product 33</t>
-  </si>
-  <si>
-    <t>Images/Product/product 34</t>
-  </si>
-  <si>
-    <t>Images/Product/product 35</t>
-  </si>
-  <si>
-    <t>Images/Product/product 36</t>
-  </si>
-  <si>
-    <t>Images/Product/product 37</t>
-  </si>
-  <si>
-    <t>Images/Product/product 38</t>
-  </si>
-  <si>
-    <t>Images/Product/product 39</t>
-  </si>
-  <si>
-    <t>Images/Product/product 40</t>
-  </si>
-  <si>
-    <t>Images/Product/product 41</t>
-  </si>
-  <si>
-    <t>Images/Product/product 42</t>
-  </si>
-  <si>
-    <t>Images/Product/product 43</t>
-  </si>
-  <si>
-    <t>Images/Product/product 44</t>
-  </si>
-  <si>
-    <t>Images/Product/product 45</t>
-  </si>
-  <si>
-    <t>Images/Product/product 46</t>
-  </si>
-  <si>
-    <t>Images/Product/product 47</t>
-  </si>
-  <si>
-    <t>Images/Product/product 48</t>
-  </si>
-  <si>
-    <t>Images/Product/product 49</t>
-  </si>
-  <si>
-    <t>Images/Product/product 50</t>
-  </si>
-  <si>
-    <t>Images/Product/product 51</t>
-  </si>
-  <si>
-    <t>Images/Product/product 52</t>
-  </si>
-  <si>
-    <t>Images/Product/product 53</t>
-  </si>
-  <si>
-    <t>Images/Product/product 54</t>
-  </si>
-  <si>
-    <t>Images/Product/product 55</t>
-  </si>
-  <si>
-    <t>Images/Product/product 56</t>
-  </si>
-  <si>
-    <t>Images/Product/product 57</t>
-  </si>
-  <si>
-    <t>Images/Product/product 58</t>
-  </si>
-  <si>
-    <t>Images/Product/product 59</t>
-  </si>
-  <si>
-    <t>Images/Product/product 60</t>
-  </si>
-  <si>
-    <t>Images/Product/product 61</t>
-  </si>
-  <si>
-    <t>Images/Product/product 62</t>
-  </si>
-  <si>
-    <t>Images/Product/product 63</t>
-  </si>
-  <si>
-    <t>Images/Product/product 64</t>
-  </si>
-  <si>
-    <t>Images/Product/product 65</t>
-  </si>
-  <si>
-    <t>Images/Product/product 66</t>
-  </si>
-  <si>
-    <t>Images/Product/product 67</t>
-  </si>
-  <si>
-    <t>Images/Product/product 68</t>
-  </si>
-  <si>
-    <t>Images/Product/product 69</t>
-  </si>
-  <si>
-    <t>Images/Product/product 70</t>
-  </si>
-  <si>
-    <t>Images/Product/product 71</t>
-  </si>
-  <si>
-    <t>Images/Product/product 72</t>
-  </si>
-  <si>
-    <t>Images/Product/product 73</t>
-  </si>
-  <si>
-    <t>Images/Product/product 74</t>
-  </si>
-  <si>
-    <t>Images/Product/product 75</t>
-  </si>
-  <si>
-    <t>Images/Product/product 76</t>
-  </si>
-  <si>
-    <t>Images/Product/product 77</t>
-  </si>
-  <si>
-    <t>Images/Product/product 78</t>
-  </si>
-  <si>
-    <t>Images/Product/product 79</t>
-  </si>
-  <si>
-    <t>Images/Product/product 80</t>
-  </si>
-  <si>
-    <t>Images/Product/product 81</t>
-  </si>
-  <si>
-    <t>Images/Product/product 82</t>
-  </si>
-  <si>
-    <t>Images/Product/product 83</t>
-  </si>
-  <si>
-    <t>Images/Product/product 84</t>
-  </si>
-  <si>
-    <t>Images/Product/product 85</t>
-  </si>
-  <si>
-    <t>Images/Product/product 86</t>
-  </si>
-  <si>
-    <t>Images/Product/product 87</t>
-  </si>
-  <si>
-    <t>Images/Product/product 88</t>
-  </si>
-  <si>
-    <t>Images/Product/product 89</t>
-  </si>
-  <si>
-    <t>Images/Product/product 90</t>
-  </si>
-  <si>
-    <t>Images/Product/product 91</t>
-  </si>
-  <si>
-    <t>Images/Product/product 92</t>
-  </si>
-  <si>
-    <t>Images/Product/product 93</t>
-  </si>
-  <si>
-    <t>Images/Product/product 94</t>
-  </si>
-  <si>
-    <t>Images/Product/product 95</t>
-  </si>
-  <si>
-    <t>Images/Product/product 96</t>
-  </si>
-  <si>
-    <t>Images/Product/product 97</t>
-  </si>
-  <si>
-    <t>Images/Product/product 98</t>
-  </si>
-  <si>
-    <t>Images/Product/product 99</t>
-  </si>
-  <si>
-    <t>Images/Product/product 100</t>
+    <t>Images/Product/product100.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product001.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product002.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product003.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product004.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product005.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product006.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product007.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product008.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product009.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product010.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product011.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product012.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product013.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product014.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product015.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product016.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product017.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product018.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product019.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product020.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product021.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product022.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product023.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product024.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product025.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product026.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product027.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product028.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product029.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product030.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product031.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product032.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product033.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product034.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product035.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product036.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product037.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product038.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product039.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product040.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product041.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product042.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product043.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product044.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product045.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product046.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product047.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product048.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product049.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product050.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product051.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product052.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product053.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product054.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product055.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product056.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product057.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product058.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product059.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product060.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product061.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product062.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product063.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product064.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product065.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product066.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product067.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product068.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product069.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product070.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product071.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product072.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product073.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product074.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product075.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product076.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product077.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product078.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product079.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product080.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product081.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product082.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product083.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product084.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product085.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product086.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product087.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product088.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product089.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product090.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product091.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product092.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product093.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product094.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product095.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product096.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product097.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product098.png</t>
+  </si>
+  <si>
+    <t>Images/Product/product099.png</t>
   </si>
 </sst>
 </file>
@@ -1160,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="C85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="C91" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1205,7 @@
         <v>458.62</v>
       </c>
       <c r="D2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1225,7 +1225,7 @@
         <v>742.6</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1245,7 +1245,7 @@
         <v>224.14</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1265,7 +1265,7 @@
         <v>681.94</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -1285,7 +1285,7 @@
         <v>634.55999999999995</v>
       </c>
       <c r="D6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1305,7 +1305,7 @@
         <v>917.06</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -1325,7 +1325,7 @@
         <v>91.08</v>
       </c>
       <c r="D8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1345,7 +1345,7 @@
         <v>668.65</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -1365,7 +1365,7 @@
         <v>800.59</v>
       </c>
       <c r="D10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -1385,7 +1385,7 @@
         <v>71.13</v>
       </c>
       <c r="D11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -1405,7 +1405,7 @@
         <v>274.27</v>
       </c>
       <c r="D12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -1425,7 +1425,7 @@
         <v>513.16999999999996</v>
       </c>
       <c r="D13" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -1445,7 +1445,7 @@
         <v>425.67</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1465,7 +1465,7 @@
         <v>29.57</v>
       </c>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1485,7 +1485,7 @@
         <v>335.37</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E16">
         <v>5</v>
@@ -1505,7 +1505,7 @@
         <v>860.97</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -1525,7 +1525,7 @@
         <v>832.49</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -1545,7 +1545,7 @@
         <v>29.88</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -1565,7 +1565,7 @@
         <v>858.53</v>
       </c>
       <c r="D20" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1585,7 +1585,7 @@
         <v>916.72</v>
       </c>
       <c r="D21" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -1605,7 +1605,7 @@
         <v>383.78</v>
       </c>
       <c r="D22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E22">
         <v>5</v>
@@ -1625,7 +1625,7 @@
         <v>737.65</v>
       </c>
       <c r="D23" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -1645,7 +1645,7 @@
         <v>674.72</v>
       </c>
       <c r="D24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -1665,7 +1665,7 @@
         <v>795.37</v>
       </c>
       <c r="D25" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1685,7 +1685,7 @@
         <v>145.94999999999999</v>
       </c>
       <c r="D26" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1705,7 +1705,7 @@
         <v>22.59</v>
       </c>
       <c r="D27" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -1725,7 +1725,7 @@
         <v>922.95</v>
       </c>
       <c r="D28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -1745,7 +1745,7 @@
         <v>673.12</v>
       </c>
       <c r="D29" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -1765,7 +1765,7 @@
         <v>202.88</v>
       </c>
       <c r="D30" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -1785,7 +1785,7 @@
         <v>705.74</v>
       </c>
       <c r="D31" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -1805,7 +1805,7 @@
         <v>537.95000000000005</v>
       </c>
       <c r="D32" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -1825,7 +1825,7 @@
         <v>522.41999999999996</v>
       </c>
       <c r="D33" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1845,7 +1845,7 @@
         <v>845.94</v>
       </c>
       <c r="D34" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E34">
         <v>3</v>
@@ -1865,7 +1865,7 @@
         <v>377.11</v>
       </c>
       <c r="D35" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -1885,7 +1885,7 @@
         <v>518.26</v>
       </c>
       <c r="D36" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E36">
         <v>5</v>
@@ -1905,7 +1905,7 @@
         <v>338.59</v>
       </c>
       <c r="D37" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -1925,7 +1925,7 @@
         <v>382.03</v>
       </c>
       <c r="D38" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E38">
         <v>3</v>
@@ -1945,7 +1945,7 @@
         <v>519.85</v>
       </c>
       <c r="D39" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -1965,7 +1965,7 @@
         <v>94.18</v>
       </c>
       <c r="D40" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E40">
         <v>4</v>
@@ -1985,7 +1985,7 @@
         <v>993.62</v>
       </c>
       <c r="D41" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -2005,7 +2005,7 @@
         <v>847.03</v>
       </c>
       <c r="D42" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E42">
         <v>3</v>
@@ -2025,7 +2025,7 @@
         <v>613.52</v>
       </c>
       <c r="D43" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E43">
         <v>2</v>
@@ -2045,7 +2045,7 @@
         <v>32</v>
       </c>
       <c r="D44" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E44">
         <v>5</v>
@@ -2065,7 +2065,7 @@
         <v>163.71</v>
       </c>
       <c r="D45" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E45">
         <v>4</v>
@@ -2085,7 +2085,7 @@
         <v>225.36</v>
       </c>
       <c r="D46" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -2105,7 +2105,7 @@
         <v>203.35</v>
       </c>
       <c r="D47" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E47">
         <v>3</v>
@@ -2125,7 +2125,7 @@
         <v>53.33</v>
       </c>
       <c r="D48" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E48">
         <v>2</v>
@@ -2145,7 +2145,7 @@
         <v>327.88</v>
       </c>
       <c r="D49" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E49">
         <v>5</v>
@@ -2165,7 +2165,7 @@
         <v>83.86</v>
       </c>
       <c r="D50" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -2185,7 +2185,7 @@
         <v>64.900000000000006</v>
       </c>
       <c r="D51" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E51">
         <v>5</v>
@@ -2205,7 +2205,7 @@
         <v>861.97</v>
       </c>
       <c r="D52" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -2225,7 +2225,7 @@
         <v>555.99</v>
       </c>
       <c r="D53" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E53">
         <v>4</v>
@@ -2245,7 +2245,7 @@
         <v>336.32</v>
       </c>
       <c r="D54" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E54">
         <v>5</v>
@@ -2265,7 +2265,7 @@
         <v>916.4</v>
       </c>
       <c r="D55" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E55">
         <v>3</v>
@@ -2285,7 +2285,7 @@
         <v>454.79</v>
       </c>
       <c r="D56" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E56">
         <v>3</v>
@@ -2305,7 +2305,7 @@
         <v>100.87</v>
       </c>
       <c r="D57" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -2325,7 +2325,7 @@
         <v>179.26</v>
       </c>
       <c r="D58" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2345,7 +2345,7 @@
         <v>61.79</v>
       </c>
       <c r="D59" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E59">
         <v>4</v>
@@ -2365,7 +2365,7 @@
         <v>37.409999999999997</v>
       </c>
       <c r="D60" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -2385,7 +2385,7 @@
         <v>23.35</v>
       </c>
       <c r="D61" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E61">
         <v>5</v>
@@ -2405,7 +2405,7 @@
         <v>136.5</v>
       </c>
       <c r="D62" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2425,7 +2425,7 @@
         <v>566.92999999999995</v>
       </c>
       <c r="D63" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -2445,7 +2445,7 @@
         <v>340.44</v>
       </c>
       <c r="D64" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E64">
         <v>2</v>
@@ -2465,7 +2465,7 @@
         <v>161.02000000000001</v>
       </c>
       <c r="D65" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E65">
         <v>4</v>
@@ -2485,7 +2485,7 @@
         <v>863.74</v>
       </c>
       <c r="D66" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E66">
         <v>3</v>
@@ -2505,7 +2505,7 @@
         <v>717.09</v>
       </c>
       <c r="D67" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E67">
         <v>3</v>
@@ -2525,7 +2525,7 @@
         <v>902.91</v>
       </c>
       <c r="D68" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E68">
         <v>5</v>
@@ -2545,7 +2545,7 @@
         <v>870.81</v>
       </c>
       <c r="D69" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E69">
         <v>3</v>
@@ -2565,7 +2565,7 @@
         <v>570.76</v>
       </c>
       <c r="D70" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -2585,7 +2585,7 @@
         <v>272.2</v>
       </c>
       <c r="D71" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -2605,7 +2605,7 @@
         <v>359.22</v>
       </c>
       <c r="D72" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2625,7 +2625,7 @@
         <v>822.64</v>
       </c>
       <c r="D73" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E73">
         <v>3</v>
@@ -2645,7 +2645,7 @@
         <v>139.88</v>
       </c>
       <c r="D74" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E74">
         <v>3</v>
@@ -2665,7 +2665,7 @@
         <v>953.44</v>
       </c>
       <c r="D75" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E75">
         <v>2</v>
@@ -2685,7 +2685,7 @@
         <v>327.14999999999998</v>
       </c>
       <c r="D76" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -2705,7 +2705,7 @@
         <v>955.21</v>
       </c>
       <c r="D77" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -2725,7 +2725,7 @@
         <v>290.89</v>
       </c>
       <c r="D78" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E78">
         <v>4</v>
@@ -2745,7 +2745,7 @@
         <v>677.61</v>
       </c>
       <c r="D79" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E79">
         <v>3</v>
@@ -2765,7 +2765,7 @@
         <v>188.17</v>
       </c>
       <c r="D80" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E80">
         <v>3</v>
@@ -2785,7 +2785,7 @@
         <v>987.03</v>
       </c>
       <c r="D81" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -2805,7 +2805,7 @@
         <v>891.25</v>
       </c>
       <c r="D82" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E82">
         <v>3</v>
@@ -2825,7 +2825,7 @@
         <v>631.1</v>
       </c>
       <c r="D83" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -2845,7 +2845,7 @@
         <v>819.88</v>
       </c>
       <c r="D84" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E84">
         <v>5</v>
@@ -2865,7 +2865,7 @@
         <v>998.73</v>
       </c>
       <c r="D85" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -2885,7 +2885,7 @@
         <v>462.31</v>
       </c>
       <c r="D86" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E86">
         <v>4</v>
@@ -2905,7 +2905,7 @@
         <v>849.7</v>
       </c>
       <c r="D87" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E87">
         <v>4</v>
@@ -2925,7 +2925,7 @@
         <v>240.36</v>
       </c>
       <c r="D88" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E88">
         <v>3</v>
@@ -2945,7 +2945,7 @@
         <v>835.51</v>
       </c>
       <c r="D89" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E89">
         <v>5</v>
@@ -2965,7 +2965,7 @@
         <v>59.41</v>
       </c>
       <c r="D90" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E90">
         <v>3</v>
@@ -2985,7 +2985,7 @@
         <v>584.84</v>
       </c>
       <c r="D91" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E91">
         <v>2</v>
@@ -3005,7 +3005,7 @@
         <v>983.75</v>
       </c>
       <c r="D92" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E92">
         <v>2</v>
@@ -3025,7 +3025,7 @@
         <v>982.99</v>
       </c>
       <c r="D93" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -3045,7 +3045,7 @@
         <v>590.34</v>
       </c>
       <c r="D94" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -3065,7 +3065,7 @@
         <v>803.68</v>
       </c>
       <c r="D95" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E95">
         <v>3</v>
@@ -3085,7 +3085,7 @@
         <v>713.22</v>
       </c>
       <c r="D96" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -3105,7 +3105,7 @@
         <v>306.29000000000002</v>
       </c>
       <c r="D97" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E97">
         <v>3</v>
@@ -3125,7 +3125,7 @@
         <v>525.22</v>
       </c>
       <c r="D98" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E98">
         <v>5</v>
@@ -3145,7 +3145,7 @@
         <v>616.66999999999996</v>
       </c>
       <c r="D99" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E99">
         <v>3</v>
@@ -3165,7 +3165,7 @@
         <v>70.44</v>
       </c>
       <c r="D100" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E100">
         <v>5</v>
@@ -3185,7 +3185,7 @@
         <v>530.21</v>
       </c>
       <c r="D101" t="s">
-        <v>264</v>
+        <v>165</v>
       </c>
       <c r="E101">
         <v>4</v>

</xml_diff>